<commit_message>
Revision of Loading your Data documentation. Corrected text, new figures.
</commit_message>
<xml_diff>
--- a/doc/visual-programming/source/loading-your-data/sample-head.xlsx
+++ b/doc/visual-programming/source/loading-your-data/sample-head.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="0" windowWidth="13920" windowHeight="8480" tabRatio="500"/>
+    <workbookView xWindow="7240" yWindow="11740" windowWidth="13920" windowHeight="8480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Untitled.tab" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
-    <t>heat 0</t>
-  </si>
-  <si>
-    <t>heat 10</t>
-  </si>
-  <si>
-    <t>heat 20</t>
-  </si>
-  <si>
-    <t>function</t>
-  </si>
-  <si>
-    <t>gene</t>
-  </si>
-  <si>
     <t>Proteas</t>
   </si>
   <si>
@@ -73,6 +58,21 @@
   </si>
   <si>
     <t>spo-mid</t>
+  </si>
+  <si>
+    <t>mD#function</t>
+  </si>
+  <si>
+    <t>mS#gene</t>
+  </si>
+  <si>
+    <t>c#heat 0</t>
+  </si>
+  <si>
+    <t>i#heat 10</t>
+  </si>
+  <si>
+    <t>i#heat 20</t>
   </si>
 </sst>
 </file>
@@ -444,40 +444,40 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0.30099999999999999</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0.20799999999999999</v>
@@ -514,10 +514,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>-0.17899999999999999</v>
@@ -534,10 +534,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>-8.5000000000000006E-2</v>
@@ -557,10 +557,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>-0.216</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
       <c r="C7">
         <v>1.7000000000000001E-2</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0.115</v>
@@ -623,10 +623,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>5.0000000000000001E-3</v>

</xml_diff>